<commit_message>
final kf faktoren michviehstall
</commit_message>
<xml_diff>
--- a/Kali_Zusammenfassung_20240813.xlsx
+++ b/Kali_Zusammenfassung_20240813.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\AG-Daten\Protokolle-SOPs\VSB_Rinderstall\Plausibilisierung\Plau_Kraftfutter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F52E4F-D099-4942-A8B8-E1D593732583}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E10069-98C9-4EAF-A51E-90CB5F411C3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{89151DBA-1DD6-46EF-BD97-ED12116356EC}"/>
   </bookViews>
@@ -564,7 +564,7 @@
   <dimension ref="A1:G1183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E1186" sqref="E1186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18429,10 +18429,10 @@
         <v>28</v>
       </c>
       <c r="E775" t="s">
+        <v>38</v>
+      </c>
+      <c r="F775" t="s">
         <v>24</v>
-      </c>
-      <c r="F775" t="s">
-        <v>38</v>
       </c>
       <c r="G775" t="s">
         <v>43</v>
@@ -27824,7 +27824,7 @@
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="B42:B852 F42:F852" name="Bereich1_1"/>
+    <protectedRange sqref="B42:B852 F42:F774 F776:F852" name="Bereich1_1"/>
     <protectedRange sqref="E73" name="Bereich1_3"/>
   </protectedRanges>
   <autoFilter ref="A1:G1183" xr:uid="{38D5CE02-B8FA-4024-B7D5-1552383288C3}"/>

</xml_diff>